<commit_message>
name filter is updated
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Yazmin\AutomationProcesses\cinepolis\CinepolisAndina\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D054DB-FFB4-42C6-B0A0-56B9A5B5BA84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04824705-5C4D-4322-BE42-8E89FFE714C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="77">
   <si>
     <t>Name</t>
   </si>
@@ -99,9 +99,6 @@
     <t>input file path for non partner file</t>
   </si>
   <si>
-    <t>BD_ENCUESTA_LARGA_GULF_Tradicio</t>
-  </si>
-  <si>
     <t>InputSheetName</t>
   </si>
   <si>
@@ -117,9 +114,6 @@
     <t>TRADICIONAL</t>
   </si>
   <si>
-    <t>BD_ENCUESTA_LARGA_GULF_VIP_Sema</t>
-  </si>
-  <si>
     <t>DirectirioFilePath</t>
   </si>
   <si>
@@ -157,24 +151,6 @@
   </si>
   <si>
     <t>/Planning/0.Shipping TS 2021/1 Directory</t>
-  </si>
-  <si>
-    <t>BDLuxuryfilePath</t>
-  </si>
-  <si>
-    <t>BDLuxurySheetName</t>
-  </si>
-  <si>
-    <t>BDPremiumfilePath</t>
-  </si>
-  <si>
-    <t>BDPremiumSheetName</t>
-  </si>
-  <si>
-    <t>BDMHESheetName</t>
-  </si>
-  <si>
-    <t>BDMHEfilePath</t>
   </si>
   <si>
     <t>DataNoBelongToCurrentWeekMailSubject</t>
@@ -282,6 +258,21 @@
   </si>
   <si>
     <t>SurveyVIP_CENTRAL AMERICASheetName</t>
+  </si>
+  <si>
+    <t>BDCentralAmericaVIPfilePath</t>
+  </si>
+  <si>
+    <t>BDCentralAmericaTradfilePath</t>
+  </si>
+  <si>
+    <t>BDCentralAmericaMcfilePath</t>
+  </si>
+  <si>
+    <t>BDAndinaVIPfilePath</t>
+  </si>
+  <si>
+    <t>BDAndinaTradfilePath</t>
   </si>
 </sst>
 </file>
@@ -800,10 +791,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D20D9A4-B24A-48FB-83BA-8E4507ED59B9}">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -828,7 +819,7 @@
         <v>22</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
         <v>24</v>
@@ -836,26 +827,26 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75">
       <c r="A4" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75">
       <c r="A5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="21" t="s">
         <v>28</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75">
@@ -864,235 +855,235 @@
     </row>
     <row r="7" spans="1:3" ht="15.75">
       <c r="A7" s="2" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="2"/>
-      <c r="B9" s="22"/>
-    </row>
-    <row r="10" spans="1:3" ht="15.75">
-      <c r="A10" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="A8" s="2"/>
+      <c r="B8" s="22"/>
+    </row>
+    <row r="9" spans="1:3" ht="15.75">
+      <c r="A9" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="2"/>
+      <c r="B10" s="22"/>
+    </row>
+    <row r="11" spans="1:3" ht="15.75">
       <c r="A11" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>74</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.75">
       <c r="A12" s="2"/>
-      <c r="B12" s="22"/>
+      <c r="B12" s="21"/>
     </row>
     <row r="13" spans="1:3" ht="15.75">
       <c r="A13" s="2" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="15.75">
-      <c r="A16" s="2" t="s">
+      <c r="A14" s="2"/>
+      <c r="B14" s="22"/>
+    </row>
+    <row r="15" spans="1:3" ht="15.75">
+      <c r="A15" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.75">
+      <c r="A17" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B17" s="21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.75">
+      <c r="A20" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15.75">
+      <c r="A23" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="2"/>
+    </row>
+    <row r="26" spans="1:2" ht="15.75">
+      <c r="A26" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="2"/>
+    </row>
+    <row r="29" spans="1:2" ht="15.75">
+      <c r="A29" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B29" s="21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B30" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="15.75">
+      <c r="A32" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32" s="21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B33" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="2"/>
+    </row>
+    <row r="35" spans="1:2" ht="15.75">
+      <c r="A35" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B35" s="23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B36" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="15.75">
-      <c r="A19" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B19" s="21" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B20" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="15.75">
-      <c r="A22" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B22" s="21" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B23" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="2"/>
-    </row>
-    <row r="25" spans="1:2" ht="15.75">
-      <c r="A25" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B25" s="21" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B26" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="2"/>
-    </row>
-    <row r="28" spans="1:2" ht="15.75">
-      <c r="A28" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B28" s="21" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B29" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="15.75">
-      <c r="A31" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B31" s="21" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B32" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="2"/>
-    </row>
-    <row r="34" spans="1:2" ht="15.75">
-      <c r="A34" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B34" s="23" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B35" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="2"/>
-    </row>
     <row r="37" spans="1:2">
-      <c r="A37" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B37" s="16">
-        <v>21</v>
-      </c>
+      <c r="A37" s="2"/>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B38" s="19" t="s">
-        <v>16</v>
+        <v>9</v>
+      </c>
+      <c r="B38" s="16">
+        <v>21</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39" s="19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B39" s="20" t="s">
+      <c r="B40" s="20" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
-      <c r="A40" s="4" t="s">
+    <row r="41" spans="1:2">
+      <c r="A41" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B40" s="20" t="s">
+      <c r="B41" s="20" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="15.75">
-      <c r="A42" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="B42" s="21" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="15.75">
       <c r="A43" s="21" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>36</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="15.75">
+      <c r="A44" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B44" s="21" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B38" r:id="rId1" xr:uid="{58EC0946-E8B4-4BDB-80EA-7ED2F2D369BC}"/>
+    <hyperlink ref="B39" r:id="rId1" xr:uid="{58EC0946-E8B4-4BDB-80EA-7ED2F2D369BC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -1181,18 +1172,18 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="24" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="24" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -1201,15 +1192,15 @@
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="24" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" s="24" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B10" s="24"/>
     </row>
@@ -1219,52 +1210,52 @@
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" s="24" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="24" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="24" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" s="24" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="18" spans="1:2" ht="14.25" customHeight="1">
       <c r="A18" s="24" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1">
       <c r="A19" s="24" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
round 1 testing done
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Yazmin\AutomationProcesses\cinepolis\CinepolisAndina\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yazmin\Documents\UiPath\cinepolisAndinaCentralAmerica\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04824705-5C4D-4322-BE42-8E89FFE714C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06340813-98EB-4A24-8D61-9AB7B4843F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="4" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="75">
   <si>
     <t>Name</t>
   </si>
@@ -108,12 +108,6 @@
     <t>InputVIPSheetName</t>
   </si>
   <si>
-    <t>LUXURY</t>
-  </si>
-  <si>
-    <t>TRADICIONAL</t>
-  </si>
-  <si>
     <t>DirectirioFilePath</t>
   </si>
   <si>
@@ -124,33 +118,6 @@
   </si>
   <si>
     <t>DirectorioSheetName</t>
-  </si>
-  <si>
-    <t>España</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS 2021/33 Envio Semana 31/ESPAÑA/TRADICIONAL</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS 2021/33 Envio Semana 31/ESPAÑA/LUXURY</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS 2021/32 Envio Semana 32</t>
-  </si>
-  <si>
-    <t>REPORTE_ESTUDIOC_CHILE_SEM_49</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS 2021/32 Envio Semana 32/CHILE/Base de Datos</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS 2021/32 Envio Semana 32/CHILE/Base de Datos/Exportadas</t>
-  </si>
-  <si>
-    <t>CHILE</t>
-  </si>
-  <si>
-    <t>/Planning/0.Shipping TS 2021/1 Directory</t>
   </si>
   <si>
     <t>DataNoBelongToCurrentWeekMailSubject</t>
@@ -197,22 +164,6 @@
 **********************This is system generated E-Mail, please do not respond on this************</t>
   </si>
   <si>
-    <t>Dear Team&lt;br/&gt;
-There is a error in Cinepolish USA run, below is the detail of error&lt;br/&gt;
-[error]&lt;br/&gt;
-Also let us know if anything is required&lt;br/&gt;
-Thank you,&lt;br/&gt;
-**********************This is system generated E-Mail, please do not respond on this************</t>
-  </si>
-  <si>
-    <t>Dear Team&lt;br/&gt;
-There is a error in Cinepos USA process run, below is the detail of error&lt;br/&gt;
-Not all required files got downloaded from FTP&lt;br/&gt;
-Also let us know if anything is required&lt;br/&gt;
-Thank you,&lt;br/&gt;
-**********************This is system generated E-Mail, please do not respond on this************</t>
-  </si>
-  <si>
     <t>WrongNameMailSubject</t>
   </si>
   <si>
@@ -273,6 +224,49 @@
   </si>
   <si>
     <t>BDAndinaTradfilePath</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS 2021/2022/03 Envio Semana 03/Andina_CENTROAMÉRICA/Bases de datos</t>
+  </si>
+  <si>
+    <t>NuevaVersion_02_2022_JUNTAS_cin</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS 2021/2022/03 Envio Semana 03/Andina_CENTROAMÉRICA/MC_CENTROAMERICA</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS 2021/2022/03 Envio Semana 03/Andina_CENTROAMÉRICA/TRADICIONAL_ANDINA</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS 2021/2022/03 Envio Semana 03/Andina_CENTROAMÉRICA/TRADICIONAL_CENTROAMERICA</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS 2021/2022/03 Envio Semana 03/Andina_CENTROAMÉRICA/VIP_ANDINA</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS 2021/2022/03 Envio Semana 03/Andina_CENTROAMÉRICA/VIP_CENTROAMERICA</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS 2021/2022/03 Envio Semana 03/Andina_CENTROAMÉRICA/Bases de datos/Exportadas</t>
+  </si>
+  <si>
+    <t>Claves Centroamérica</t>
+  </si>
+  <si>
+    <t>Dear Team&lt;br/&gt;
+There is an error in Cinepolish andina run, below is the detail of error&lt;br/&gt;
+[error]&lt;br/&gt;
+Also let us know if anything is required&lt;br/&gt;
+Thank you,&lt;br/&gt;
+**********************This is system generated E-Mail, please do not respond on this************</t>
+  </si>
+  <si>
+    <t>Dear Team&lt;br/&gt;
+There is an error in Cinepos andina process run, below is the detail of error&lt;br/&gt;
+Not all required files got downloaded from FTP&lt;br/&gt;
+Also let us know if anything is required&lt;br/&gt;
+Thank you,&lt;br/&gt;
+**********************This is system generated E-Mail, please do not respond on this************</t>
   </si>
 </sst>
 </file>
@@ -793,13 +787,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D20D9A4-B24A-48FB-83BA-8E4507ED59B9}">
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="84.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -819,7 +813,7 @@
         <v>22</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
         <v>24</v>
@@ -830,35 +824,31 @@
         <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75">
       <c r="A4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="21" t="s">
-        <v>29</v>
-      </c>
+      <c r="B4" s="21"/>
     </row>
     <row r="5" spans="1:3" ht="15.75">
       <c r="A5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="21" t="s">
-        <v>28</v>
-      </c>
+      <c r="B5" s="21"/>
     </row>
     <row r="6" spans="1:3" ht="15.75">
       <c r="A6" s="2"/>
       <c r="B6" s="21"/>
     </row>
-    <row r="7" spans="1:3" ht="15.75">
+    <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>36</v>
+        <v>59</v>
+      </c>
+      <c r="B7" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -867,10 +857,10 @@
     </row>
     <row r="9" spans="1:3" ht="15.75">
       <c r="A9" s="2" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -879,10 +869,10 @@
     </row>
     <row r="11" spans="1:3" ht="15.75">
       <c r="A11" s="2" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75">
@@ -891,10 +881,10 @@
     </row>
     <row r="13" spans="1:3" ht="15.75">
       <c r="A13" s="2" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>36</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -903,10 +893,10 @@
     </row>
     <row r="15" spans="1:3" ht="15.75">
       <c r="A15" s="2" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15.75">
@@ -914,7 +904,7 @@
         <v>8</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -927,15 +917,15 @@
     </row>
     <row r="20" spans="1:2" ht="15.75">
       <c r="A20" s="2" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>40</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="2" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="B21" t="s">
         <v>14</v>
@@ -943,15 +933,15 @@
     </row>
     <row r="23" spans="1:2" ht="15.75">
       <c r="A23" s="2" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>40</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="2" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="B24" t="s">
         <v>14</v>
@@ -962,15 +952,15 @@
     </row>
     <row r="26" spans="1:2" ht="15.75">
       <c r="A26" s="2" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>40</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="2" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="B27" t="s">
         <v>14</v>
@@ -981,15 +971,15 @@
     </row>
     <row r="29" spans="1:2" ht="15.75">
       <c r="A29" s="2" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>40</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="2" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B30" t="s">
         <v>14</v>
@@ -997,15 +987,15 @@
     </row>
     <row r="32" spans="1:2" ht="15.75">
       <c r="A32" s="2" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="B32" s="21" t="s">
-        <v>40</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="2" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="B33" t="s">
         <v>14</v>
@@ -1016,18 +1006,18 @@
     </row>
     <row r="35" spans="1:2" ht="15.75">
       <c r="A35" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B35" s="23" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B36" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1067,18 +1057,18 @@
     </row>
     <row r="43" spans="1:2" ht="15.75">
       <c r="A43" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="B43" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B43" s="23" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="15.75">
       <c r="A44" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="B44" s="21" t="s">
-        <v>34</v>
+        <v>31</v>
+      </c>
+      <c r="B44" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1094,8 +1084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z978"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1172,18 +1162,18 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="24" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="24" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -1192,15 +1182,15 @@
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="24" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" s="24" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="B10" s="24"/>
     </row>
@@ -1210,52 +1200,52 @@
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" s="24" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="24" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="24" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" s="24" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="18" spans="1:2" ht="14.25" customHeight="1">
       <c r="A18" s="24" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1">
       <c r="A19" s="24" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
input file changes done
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yazmin\Documents\UiPath\cinepolisAndinaCentralAmerica\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06340813-98EB-4A24-8D61-9AB7B4843F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC0C013-4F67-4650-9147-EE1EC7F61D5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="79">
   <si>
     <t>Name</t>
   </si>
@@ -91,9 +91,6 @@
   </si>
   <si>
     <t>InputnonPartnerFilePath</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS 2021/1 Directorio</t>
   </si>
   <si>
     <t>input file path for non partner file</t>
@@ -267,6 +264,21 @@
 Also let us know if anything is required&lt;br/&gt;
 Thank you,&lt;br/&gt;
 **********************This is system generated E-Mail, please do not respond on this************</t>
+  </si>
+  <si>
+    <t>arerodriguez@tecnoyar.com</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS 2021/2022/03 Envio Semana 03/MÉXICO/Base de Datos</t>
+  </si>
+  <si>
+    <t>WorkingStartDate</t>
+  </si>
+  <si>
+    <t>dd/MM/yyyy</t>
+  </si>
+  <si>
+    <t>WorkingEndDate</t>
   </si>
 </sst>
 </file>
@@ -423,7 +435,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -470,6 +482,9 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -787,8 +802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D20D9A4-B24A-48FB-83BA-8E4507ED59B9}">
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -813,29 +828,29 @@
         <v>22</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75">
       <c r="A4" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="21"/>
     </row>
     <row r="5" spans="1:3" ht="15.75">
       <c r="A5" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="21"/>
     </row>
@@ -845,10 +860,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -857,10 +872,10 @@
     </row>
     <row r="9" spans="1:3" ht="15.75">
       <c r="A9" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -869,10 +884,10 @@
     </row>
     <row r="11" spans="1:3" ht="15.75">
       <c r="A11" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75">
@@ -881,10 +896,10 @@
     </row>
     <row r="13" spans="1:3" ht="15.75">
       <c r="A13" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -893,10 +908,10 @@
     </row>
     <row r="15" spans="1:3" ht="15.75">
       <c r="A15" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15.75">
@@ -904,7 +919,7 @@
         <v>8</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -917,15 +932,15 @@
     </row>
     <row r="20" spans="1:2" ht="15.75">
       <c r="A20" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B21" t="s">
         <v>14</v>
@@ -933,15 +948,15 @@
     </row>
     <row r="23" spans="1:2" ht="15.75">
       <c r="A23" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B24" t="s">
         <v>14</v>
@@ -952,15 +967,15 @@
     </row>
     <row r="26" spans="1:2" ht="15.75">
       <c r="A26" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B27" t="s">
         <v>14</v>
@@ -971,15 +986,15 @@
     </row>
     <row r="29" spans="1:2" ht="15.75">
       <c r="A29" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B30" t="s">
         <v>14</v>
@@ -987,15 +1002,15 @@
     </row>
     <row r="32" spans="1:2" ht="15.75">
       <c r="A32" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B32" s="21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B33" t="s">
         <v>14</v>
@@ -1006,18 +1021,18 @@
     </row>
     <row r="35" spans="1:2" ht="15.75">
       <c r="A35" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B35" s="23" t="s">
-        <v>23</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B36" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1057,18 +1072,18 @@
     </row>
     <row r="43" spans="1:2" ht="15.75">
       <c r="A43" s="21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B43" s="23" t="s">
-        <v>23</v>
+        <v>75</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="15.75">
       <c r="A44" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B44" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1084,8 +1099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z978"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1162,18 +1177,18 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="24" t="s">
         <v>32</v>
-      </c>
-      <c r="B6" s="24" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -1182,17 +1197,19 @@
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="27" t="s">
         <v>35</v>
-      </c>
-      <c r="B9" s="27" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="24"/>
+        <v>36</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" s="24"/>
@@ -1200,67 +1217,87 @@
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="24" t="s">
         <v>38</v>
-      </c>
-      <c r="B12" s="24" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="18" spans="1:2" ht="14.25" customHeight="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="24" t="s">
+    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A19" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="25" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A19" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19" s="25" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="29" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A21" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" s="29">
+        <v>44571</v>
+      </c>
+      <c r="C21" s="29" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A22" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="B22" s="29">
+        <v>44577</v>
+      </c>
+      <c r="C22" s="30" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -2211,9 +2248,10 @@
   <phoneticPr fontId="2"/>
   <hyperlinks>
     <hyperlink ref="B9" r:id="rId1" xr:uid="{B1018490-FE45-47D5-A281-E8373B4E93A6}"/>
+    <hyperlink ref="B10" r:id="rId2" xr:uid="{5B7B8B83-A9B2-44E6-ACC0-78A56F7F4815}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
changed the file logic
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Yazmin\AutomationProcesses\cinepolis\CinepolisAndina\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yazmin\Documents\UiPath\cinepolisAndinaCentralAmerica\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B8E2DC6-5B05-4F00-9E06-3785091F9B09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C08CBE-4FB2-41D0-8434-B49DEBEDFE44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="4" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="79">
   <si>
     <t>Name</t>
   </si>
@@ -103,12 +103,6 @@
   </si>
   <si>
     <t>InputVIPSheetName</t>
-  </si>
-  <si>
-    <t>DirectirioFilePath</t>
-  </si>
-  <si>
-    <t>DirectirioSheetName</t>
   </si>
   <si>
     <t>DirectorioFilePath</t>
@@ -206,9 +200,6 @@
     <t>BDAndinaTradfilePath</t>
   </si>
   <si>
-    <t>Claves Centroamérica</t>
-  </si>
-  <si>
     <t>Dear Team&lt;br/&gt;
 There is an error in Cinepolish andina run, below is the detail of error&lt;br/&gt;
 [error]&lt;br/&gt;
@@ -237,28 +228,7 @@
     <t>WorkingEndDate</t>
   </si>
   <si>
-    <t>/Planeacion/0.Envios TS/2022/04 Envio Semana 04/Andina_CENTROAMÉRICA/Bases de datos</t>
-  </si>
-  <si>
     <t>NuevaVersion_03_2022_JUNTAS_cin</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/04 Envio Semana 04/Andina_CENTROAMÉRICA/VIP_CENTROAMERICA</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/04 Envio Semana 04/Andina_CENTROAMÉRICA/TRADICIONAL_CENTROAMERICA</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/04 Envio Semana 04/Andina_CENTROAMÉRICA/MC_CENTROAMERICA</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/04 Envio Semana 04/Andina_CENTROAMÉRICA/VIP_ANDINA</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/04 Envio Semana 04/Andina_CENTROAMÉRICA/TRADICIONAL_ANDINA</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/04 Envio Semana 04/Andina_CENTROAMÉRICA/Bases de datos/Exportadas</t>
   </si>
   <si>
     <t>/Planeacion/0.Envios TS/1 Directorio</t>
@@ -279,12 +249,42 @@
 Thank you,&lt;br/&gt;
 **********************This is system generated E-Mail, please do not respond on this************</t>
   </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/05 Envio Semana 05/Andina_CENTROAMÉRICA/Bases de datos</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/05 Envio Semana 05/Andina_CENTROAMÉRICA/VIP_CENTROAMERICA</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/05 Envio Semana 05/Andina_CENTROAMÉRICA/TRADICIONAL_CENTROAMERICA</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/05 Envio Semana 05/Andina_CENTROAMÉRICA/MC_CENTROAMERICA</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/05 Envio Semana 05/Andina_CENTROAMÉRICA/VIP_ANDINA</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/05 Envio Semana 05/Andina_CENTROAMÉRICA/TRADICIONAL_ANDINA</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/05 Envio Semana 05/Andina_CENTROAMÉRICA/Bases de datos/Exportadas</t>
+  </si>
+  <si>
+    <t>Keywords in file name</t>
+  </si>
+  <si>
+    <t>nuevaversion,LATAM</t>
+  </si>
+  <si>
+    <t>Claves Centroamérica_Andina</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -412,6 +412,13 @@
       <color theme="10"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -434,7 +441,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -484,6 +491,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -799,19 +807,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D20D9A4-B24A-48FB-83BA-8E4507ED59B9}">
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:XFD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="40.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="84.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="107.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75">
+    <row r="1" spans="1:4" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -821,104 +831,113 @@
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75">
+      <c r="D1" s="31" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75">
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75">
       <c r="A4" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B4" s="21"/>
     </row>
-    <row r="5" spans="1:3" ht="15.75">
+    <row r="5" spans="1:4" ht="15.75">
       <c r="A5" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B5" s="21"/>
     </row>
-    <row r="6" spans="1:3" ht="15.75">
+    <row r="6" spans="1:4" ht="15.75">
       <c r="A6" s="2"/>
       <c r="B6" s="21"/>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="2"/>
       <c r="B8" s="22"/>
     </row>
-    <row r="9" spans="1:3" ht="15.75">
+    <row r="9" spans="1:4" ht="15.75">
       <c r="A9" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="2"/>
       <c r="B10" s="22"/>
     </row>
-    <row r="11" spans="1:3" ht="15.75">
+    <row r="11" spans="1:4" ht="15.75">
       <c r="A11" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="15.75">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.75">
       <c r="A12" s="2"/>
       <c r="B12" s="21"/>
     </row>
-    <row r="13" spans="1:3" ht="15.75">
+    <row r="13" spans="1:4" ht="15.75">
       <c r="A13" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="2"/>
       <c r="B14" s="22"/>
     </row>
-    <row r="15" spans="1:3" ht="15.75">
+    <row r="15" spans="1:4" ht="15.75">
       <c r="A15" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>72</v>
-      </c>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75">
+      <c r="B16" s="21"/>
     </row>
     <row r="17" spans="1:2" ht="15.75">
       <c r="A17" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -931,15 +950,15 @@
     </row>
     <row r="20" spans="1:2" ht="15.75">
       <c r="A20" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B21" t="s">
         <v>14</v>
@@ -947,15 +966,15 @@
     </row>
     <row r="23" spans="1:2" ht="15.75">
       <c r="A23" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B24" t="s">
         <v>14</v>
@@ -966,15 +985,15 @@
     </row>
     <row r="26" spans="1:2" ht="15.75">
       <c r="A26" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B27" t="s">
         <v>14</v>
@@ -985,15 +1004,15 @@
     </row>
     <row r="29" spans="1:2" ht="15.75">
       <c r="A29" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B30" t="s">
         <v>14</v>
@@ -1001,15 +1020,15 @@
     </row>
     <row r="32" spans="1:2" ht="15.75">
       <c r="A32" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B32" s="21" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B33" t="s">
         <v>14</v>
@@ -1018,76 +1037,60 @@
     <row r="34" spans="1:2">
       <c r="A34" s="2"/>
     </row>
-    <row r="35" spans="1:2" ht="15.75">
-      <c r="A35" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B35" s="23" t="s">
-        <v>74</v>
-      </c>
+    <row r="35" spans="1:2">
+      <c r="A35" s="2"/>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B36" t="s">
-        <v>59</v>
+        <v>9</v>
+      </c>
+      <c r="B36" s="16">
+        <v>21</v>
       </c>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" s="2"/>
+      <c r="A37" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37" s="19" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B38" s="16">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="B38" s="20" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B39" s="19" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
-      <c r="A40" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B40" s="20" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
-      <c r="A41" s="4" t="s">
+      <c r="A39" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B41" s="20" t="s">
+      <c r="B39" s="20" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="15.75">
-      <c r="A43" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="B43" s="23" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="15.75">
-      <c r="A44" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="B44" t="s">
-        <v>59</v>
+    <row r="41" spans="1:2" ht="15.75">
+      <c r="A41" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B41" s="23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="15.75">
+      <c r="A42" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B42" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B39" r:id="rId1" xr:uid="{58EC0946-E8B4-4BDB-80EA-7ED2F2D369BC}"/>
+    <hyperlink ref="B37" r:id="rId1" xr:uid="{58EC0946-E8B4-4BDB-80EA-7ED2F2D369BC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -1099,7 +1102,7 @@
   <dimension ref="A1:Z978"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1176,18 +1179,18 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="24" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="24" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -1196,18 +1199,18 @@
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="24" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" s="24" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -1216,75 +1219,75 @@
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" s="24" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="24" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="24" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" s="24" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" s="24" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" s="24" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B21" s="29">
-        <v>44578</v>
+        <v>44585</v>
       </c>
       <c r="C21" s="29" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" s="24" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B22" s="29">
-        <v>44584</v>
+        <v>44591</v>
       </c>
       <c r="C22" s="30" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
process updated with encoding "iso-8859-15"
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yazmin\Documents\UiPath\cinepolisAndinaCentralAmerica\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE3EA2FA-36E8-4429-9367-5548EA1F07A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DFBC511-FABC-4EBD-A351-5F12B956D629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="4" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="83">
   <si>
     <t>Name</t>
   </si>
@@ -228,9 +228,6 @@
     <t>WorkingEndDate</t>
   </si>
   <si>
-    <t>NuevaVersion_03_2022_JUNTAS_cin</t>
-  </si>
-  <si>
     <t>/Planeacion/0.Envios TS/1 Directorio</t>
   </si>
   <si>
@@ -250,27 +247,6 @@
 **********************This is system generated E-Mail, please do not respond on this************</t>
   </si>
   <si>
-    <t>/Planeacion/0.Envios TS/2022/05 Envio Semana 05/Andina_CENTROAMÉRICA/Bases de datos</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/05 Envio Semana 05/Andina_CENTROAMÉRICA/VIP_CENTROAMERICA</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/05 Envio Semana 05/Andina_CENTROAMÉRICA/TRADICIONAL_CENTROAMERICA</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/05 Envio Semana 05/Andina_CENTROAMÉRICA/MC_CENTROAMERICA</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/05 Envio Semana 05/Andina_CENTROAMÉRICA/VIP_ANDINA</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/05 Envio Semana 05/Andina_CENTROAMÉRICA/TRADICIONAL_ANDINA</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/05 Envio Semana 05/Andina_CENTROAMÉRICA/Bases de datos/Exportadas</t>
-  </si>
-  <si>
     <t>Keywords in file name</t>
   </si>
   <si>
@@ -284,6 +260,36 @@
   </si>
   <si>
     <t>CorrectnameFilePath</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/07 Envío Semana 07/Andina_CENTROAMÉRICA/Bases de datos</t>
+  </si>
+  <si>
+    <t>NuevaVersion_06_2022_JUNTAS_cin</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/07 Envío Semana 07/Andina_CENTROAMÉRICA/Bases de datos/Exportadas</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/07 Envío Semana 07/Andina_CENTROAMÉRICA/VIP_ANDINA</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/07 Envío Semana 07/Andina_CENTROAMÉRICA/VIP_CENTROAMERICA</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/07 Envío Semana 07/Andina_CENTROAMÉRICA/TRADICIONAL_CENTROAMERICA</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/07 Envío Semana 07/Andina_CENTROAMÉRICA/TRADICIONAL_ANDINA</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/07 Envío Semana 07/Andina_CENTROAMÉRICA/MC_CENTROAMERICA</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/1 Directorio/Correcciones</t>
+  </si>
+  <si>
+    <t>Hoja</t>
   </si>
 </sst>
 </file>
@@ -815,8 +821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D20D9A4-B24A-48FB-83BA-8E4507ED59B9}">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -838,7 +844,7 @@
         <v>3</v>
       </c>
       <c r="D1" s="31" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75">
@@ -846,13 +852,13 @@
         <v>22</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C2" t="s">
         <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -860,7 +866,7 @@
         <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75">
@@ -884,7 +890,7 @@
         <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -896,7 +902,7 @@
         <v>53</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -908,7 +914,7 @@
         <v>54</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75">
@@ -920,7 +926,7 @@
         <v>55</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -932,7 +938,7 @@
         <v>56</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.75">
@@ -943,7 +949,7 @@
         <v>8</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1083,7 +1089,7 @@
         <v>27</v>
       </c>
       <c r="B41" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15.75">
@@ -1091,17 +1097,23 @@
         <v>28</v>
       </c>
       <c r="B42" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>80</v>
+        <v>72</v>
+      </c>
+      <c r="B44" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>79</v>
+        <v>71</v>
+      </c>
+      <c r="B45" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1117,7 +1129,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z978"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -1269,18 +1281,18 @@
     <row r="17" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" s="24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" s="25" t="s">
         <v>67</v>
-      </c>
-      <c r="B19" s="25" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
@@ -1289,7 +1301,7 @@
         <v>60</v>
       </c>
       <c r="B21" s="29">
-        <v>44585</v>
+        <v>44599</v>
       </c>
       <c r="C21" s="29" t="s">
         <v>61</v>
@@ -1300,7 +1312,7 @@
         <v>62</v>
       </c>
       <c r="B22" s="29">
-        <v>44591</v>
+        <v>44605</v>
       </c>
       <c r="C22" s="30" t="s">
         <v>61</v>

</xml_diff>